<commit_message>
replaced Eulophid sp. A with Tetrastichs sp.
I also included some speculative information on its biology
</commit_message>
<xml_diff>
--- a/parasitoid_biology.xlsx
+++ b/parasitoid_biology.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Iteomyia,                  R. salicisbrassicoides, R. salicisbattatus</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -90,19 +90,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Mymarid sp. A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Mymaridae</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>egg</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>NA</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -225,10 +217,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Eulophid sp. A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Eulophidae</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -273,12 +261,38 @@
     <t>Ichneumonidae</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>Tetrastichus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> sp.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mymarid sp. A</t>
+  </si>
+  <si>
+    <t>Idiobiont, ectoparasitoid?</t>
+  </si>
+  <si>
+    <t>late-instar larvae?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -310,7 +324,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -320,35 +334,24 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,12 +369,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -694,14 +700,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="3" width="11.85546875" customWidth="1"/>
@@ -713,42 +719,42 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39">
       <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>0</v>
@@ -758,43 +764,43 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="26">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="26">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>10</v>
@@ -805,19 +811,19 @@
     </row>
     <row r="5" spans="1:7" ht="39">
       <c r="A5" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>1</v>
@@ -826,44 +832,44 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26">
-      <c r="A6" s="6" t="s">
-        <v>42</v>
+    <row r="6" spans="1:7" ht="39">
+      <c r="A6" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>7</v>
@@ -874,42 +880,42 @@
     </row>
     <row r="8" spans="1:7" ht="26">
       <c r="A8" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="26">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>9</v>
@@ -922,12 +928,11 @@
       <c r="A10" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>